<commit_message>
adapt comparison excel, create uml profile
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Papers\ECMFA_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ABFE284-BD1A-4612-AB6C-6DBFDF59A6EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0CD2DA1-E28F-4F79-93C6-82ADE2AA6D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="17520" windowHeight="12600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="262">
   <si>
     <t>Vergleichskriterien/Features</t>
   </si>
@@ -808,6 +808,12 @@
   </si>
   <si>
     <t>ownedComment</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Parameter.type</t>
   </si>
 </sst>
 </file>
@@ -5322,8 +5328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5454,7 +5460,9 @@
       <c r="C4" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="D4" s="45"/>
+      <c r="D4" s="45" t="s">
+        <v>229</v>
+      </c>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
@@ -5488,7 +5496,9 @@
       <c r="C5" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="D5" s="45"/>
+      <c r="D5" s="45" t="s">
+        <v>260</v>
+      </c>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
@@ -7314,7 +7324,9 @@
       <c r="C56" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="D56" s="45"/>
+      <c r="D56" s="45" t="s">
+        <v>261</v>
+      </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
       <c r="G56" s="8"/>

</xml_diff>

<commit_message>
update eclipse-mm and comparison excel
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ac138120\Documents\projects\dt_language_comparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Papers\ECMFA_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8D2028-D7C3-49B3-8D2D-B4962F87F92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B17188F-798E-433B-9F49-6AFE1BDE04E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="16080" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="17520" windowHeight="12600" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabellenblatt1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="340">
   <si>
     <t>Vergleichskriterien/Features</t>
   </si>
@@ -1055,6 +1055,12 @@
   <si>
     <t>Composition</t>
   </si>
+  <si>
+    <t>Association[isComposition=true]</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
 </sst>
 </file>
 
@@ -1171,7 +1177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -1560,11 +1566,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1713,10 +1732,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1748,9 +1763,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1762,6 +1774,33 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="36" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -60788,53 +60827,53 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81660679-4C16-4328-828C-2DD56627BD9C}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="109" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="113" t="s">
+      <c r="B1" s="110" t="s">
         <v>301</v>
       </c>
-      <c r="C1" s="114" t="s">
+      <c r="C1" s="111" t="s">
         <v>302</v>
       </c>
-      <c r="D1" s="114" t="s">
+      <c r="D1" s="111" t="s">
         <v>303</v>
       </c>
-      <c r="E1" s="114" t="s">
+      <c r="E1" s="111" t="s">
         <v>304</v>
       </c>
       <c r="F1" s="86"/>
     </row>
     <row r="2" spans="1:6" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="109" t="s">
+      <c r="A2" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="B2" s="110" t="s">
+      <c r="B2" s="107" t="s">
         <v>223</v>
       </c>
-      <c r="C2" s="111" t="s">
+      <c r="C2" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="111" t="s">
+      <c r="D2" s="108" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="111" t="s">
+      <c r="E2" s="108" t="s">
         <v>75</v>
       </c>
       <c r="F2" s="86"/>
@@ -60843,7 +60882,7 @@
       <c r="A3" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="96" t="s">
         <v>225</v>
       </c>
       <c r="C3" s="87" t="s">
@@ -60861,7 +60900,7 @@
       <c r="A4" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="B4" s="99" t="s">
+      <c r="B4" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="87" t="s">
@@ -60879,7 +60918,7 @@
       <c r="A5" s="84" t="s">
         <v>255</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="96" t="s">
         <v>255</v>
       </c>
       <c r="C5" s="87" t="s">
@@ -60897,7 +60936,7 @@
       <c r="A6" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="B6" s="100" t="s">
+      <c r="B6" s="98" t="s">
         <v>226</v>
       </c>
       <c r="C6" s="87" t="s">
@@ -60915,7 +60954,7 @@
       <c r="A7" s="84" t="s">
         <v>296</v>
       </c>
-      <c r="B7" s="100" t="s">
+      <c r="B7" s="98" t="s">
         <v>227</v>
       </c>
       <c r="C7" s="87" t="s">
@@ -60933,7 +60972,7 @@
       <c r="A8" s="86" t="s">
         <v>271</v>
       </c>
-      <c r="B8" s="100" t="s">
+      <c r="B8" s="98" t="s">
         <v>305</v>
       </c>
       <c r="C8" s="87" t="s">
@@ -60951,7 +60990,7 @@
       <c r="A9" s="84" t="s">
         <v>297</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="87" t="s">
@@ -60969,7 +61008,7 @@
       <c r="A10" s="86" t="s">
         <v>272</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C10" s="88" t="s">
@@ -60987,7 +61026,7 @@
       <c r="A11" s="84" t="s">
         <v>258</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C11" s="88" t="s">
@@ -61005,7 +61044,7 @@
       <c r="A12" s="84" t="s">
         <v>273</v>
       </c>
-      <c r="B12" s="100" t="s">
+      <c r="B12" s="98" t="s">
         <v>242</v>
       </c>
       <c r="C12" s="87" t="s">
@@ -61023,7 +61062,7 @@
       <c r="A13" s="84" t="s">
         <v>336</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C13" s="87"/>
@@ -61036,44 +61075,44 @@
       <c r="F13" s="86"/>
     </row>
     <row r="14" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="106" t="s">
+      <c r="A14" s="103" t="s">
         <v>335</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="99" t="s">
         <v>335</v>
       </c>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92" t="s">
+      <c r="C14" s="90"/>
+      <c r="D14" s="90" t="s">
         <v>335</v>
       </c>
-      <c r="E14" s="93" t="s">
+      <c r="E14" s="91" t="s">
         <v>23</v>
       </c>
       <c r="F14" s="86"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="107" t="s">
+      <c r="A15" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="95" t="s">
+      <c r="C15" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="95" t="s">
+      <c r="D15" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="95" t="s">
+      <c r="E15" s="93" t="s">
         <v>148</v>
       </c>
       <c r="F15" s="86"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="108" t="s">
+      <c r="A16" s="105" t="s">
         <v>293</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="101" t="s">
         <v>240</v>
       </c>
       <c r="C16" s="87" t="s">
@@ -61091,7 +61130,7 @@
       <c r="A17" s="84" t="s">
         <v>294</v>
       </c>
-      <c r="B17" s="99" t="s">
+      <c r="B17" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C17" s="88" t="s">
@@ -61109,7 +61148,7 @@
       <c r="A18" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="103"/>
+      <c r="B18" s="101"/>
       <c r="C18" s="87" t="s">
         <v>61</v>
       </c>
@@ -61125,7 +61164,7 @@
       <c r="A19" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="B19" s="100" t="s">
+      <c r="B19" s="98" t="s">
         <v>225</v>
       </c>
       <c r="C19" s="87" t="s">
@@ -61143,7 +61182,7 @@
       <c r="A20" s="86" t="s">
         <v>274</v>
       </c>
-      <c r="B20" s="99" t="s">
+      <c r="B20" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="88" t="s">
@@ -61161,7 +61200,7 @@
       <c r="A21" s="86" t="s">
         <v>275</v>
       </c>
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C21" s="88" t="s">
@@ -61179,7 +61218,7 @@
       <c r="A22" s="86" t="s">
         <v>262</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="88" t="s">
@@ -61197,7 +61236,7 @@
       <c r="A23" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="B23" s="98" t="s">
+      <c r="B23" s="96" t="s">
         <v>232</v>
       </c>
       <c r="C23" s="88" t="s">
@@ -61215,7 +61254,7 @@
       <c r="A24" s="86" t="s">
         <v>276</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="88" t="s">
@@ -61233,7 +61272,7 @@
       <c r="A25" s="84" t="s">
         <v>277</v>
       </c>
-      <c r="B25" s="99" t="s">
+      <c r="B25" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="87" t="s">
@@ -61251,7 +61290,7 @@
       <c r="A26" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="B26" s="98" t="s">
+      <c r="B26" s="96" t="s">
         <v>226</v>
       </c>
       <c r="C26" s="87" t="s">
@@ -61269,7 +61308,7 @@
       <c r="A27" s="86" t="s">
         <v>279</v>
       </c>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="96" t="s">
         <v>233</v>
       </c>
       <c r="C27" s="88" t="s">
@@ -61287,7 +61326,7 @@
       <c r="A28" s="86" t="s">
         <v>281</v>
       </c>
-      <c r="B28" s="98" t="s">
+      <c r="B28" s="96" t="s">
         <v>236</v>
       </c>
       <c r="C28" s="88" t="s">
@@ -61305,7 +61344,7 @@
       <c r="A29" s="86" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="98" t="s">
+      <c r="B29" s="96" t="s">
         <v>237</v>
       </c>
       <c r="C29" s="88" t="s">
@@ -61323,7 +61362,7 @@
       <c r="A30" s="86" t="s">
         <v>282</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="96" t="s">
         <v>240</v>
       </c>
       <c r="C30" s="88" t="s">
@@ -61341,7 +61380,7 @@
       <c r="A31" s="86" t="s">
         <v>280</v>
       </c>
-      <c r="B31" s="99" t="s">
+      <c r="B31" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C31" s="87" t="s">
@@ -61359,7 +61398,7 @@
       <c r="A32" s="84" t="s">
         <v>270</v>
       </c>
-      <c r="B32" s="103" t="s">
+      <c r="B32" s="101" t="s">
         <v>257</v>
       </c>
       <c r="C32" s="87" t="s">
@@ -61377,7 +61416,7 @@
       <c r="A33" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="B33" s="99" t="s">
+      <c r="B33" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C33" s="87" t="s">
@@ -61395,7 +61434,7 @@
       <c r="A34" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="B34" s="98" t="s">
+      <c r="B34" s="96" t="s">
         <v>226</v>
       </c>
       <c r="C34" s="87" t="s">
@@ -61413,7 +61452,7 @@
       <c r="A35" s="84" t="s">
         <v>296</v>
       </c>
-      <c r="B35" s="99" t="s">
+      <c r="B35" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C35" s="87" t="s">
@@ -61431,7 +61470,7 @@
       <c r="A36" s="86" t="s">
         <v>271</v>
       </c>
-      <c r="B36" s="103" t="s">
+      <c r="B36" s="101" t="s">
         <v>241</v>
       </c>
       <c r="C36" s="87" t="s">
@@ -61446,37 +61485,37 @@
       <c r="F36" s="86"/>
     </row>
     <row r="37" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="94" t="s">
+      <c r="A37" s="92" t="s">
         <v>297</v>
       </c>
-      <c r="B37" s="101" t="s">
+      <c r="B37" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="92" t="s">
+      <c r="C37" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="D37" s="92" t="s">
+      <c r="D37" s="90" t="s">
         <v>297</v>
       </c>
-      <c r="E37" s="93" t="s">
+      <c r="E37" s="91" t="s">
         <v>23</v>
       </c>
       <c r="F37" s="86"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="97" t="s">
+      <c r="A38" s="95" t="s">
         <v>283</v>
       </c>
-      <c r="B38" s="104" t="s">
+      <c r="B38" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="95" t="s">
+      <c r="C38" s="93" t="s">
         <v>98</v>
       </c>
-      <c r="D38" s="95" t="s">
+      <c r="D38" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="95" t="s">
+      <c r="E38" s="93" t="s">
         <v>88</v>
       </c>
       <c r="F38" s="86"/>
@@ -61485,7 +61524,7 @@
       <c r="A39" s="86" t="s">
         <v>284</v>
       </c>
-      <c r="B39" s="98" t="s">
+      <c r="B39" s="96" t="s">
         <v>245</v>
       </c>
       <c r="C39" s="87" t="s">
@@ -61503,7 +61542,7 @@
       <c r="A40" s="86" t="s">
         <v>285</v>
       </c>
-      <c r="B40" s="98" t="s">
+      <c r="B40" s="96" t="s">
         <v>246</v>
       </c>
       <c r="C40" s="87" t="s">
@@ -61521,7 +61560,7 @@
       <c r="A41" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="B41" s="99" t="s">
+      <c r="B41" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C41" s="88" t="s">
@@ -61539,7 +61578,7 @@
       <c r="A42" s="86" t="s">
         <v>278</v>
       </c>
-      <c r="B42" s="99" t="s">
+      <c r="B42" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C42" s="88" t="s">
@@ -61557,7 +61596,7 @@
       <c r="A43" s="86" t="s">
         <v>262</v>
       </c>
-      <c r="B43" s="99" t="s">
+      <c r="B43" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C43" s="88" t="s">
@@ -61575,7 +61614,7 @@
       <c r="A44" s="86" t="s">
         <v>286</v>
       </c>
-      <c r="B44" s="99" t="s">
+      <c r="B44" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C44" s="88" t="s">
@@ -61593,7 +61632,7 @@
       <c r="A45" s="84" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="98" t="s">
+      <c r="B45" s="96" t="s">
         <v>225</v>
       </c>
       <c r="C45" s="87" t="s">
@@ -61611,7 +61650,7 @@
       <c r="A46" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="B46" s="99" t="s">
+      <c r="B46" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C46" s="87" t="s">
@@ -61629,7 +61668,7 @@
       <c r="A47" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="B47" s="99" t="s">
+      <c r="B47" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C47" s="87" t="s">
@@ -61647,7 +61686,7 @@
       <c r="A48" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="B48" s="98" t="s">
+      <c r="B48" s="96" t="s">
         <v>226</v>
       </c>
       <c r="C48" s="87" t="s">
@@ -61665,7 +61704,7 @@
       <c r="A49" s="86" t="s">
         <v>263</v>
       </c>
-      <c r="B49" s="99" t="s">
+      <c r="B49" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C49" s="88" t="s">
@@ -61683,7 +61722,7 @@
       <c r="A50" s="86" t="s">
         <v>273</v>
       </c>
-      <c r="B50" s="98" t="s">
+      <c r="B50" s="96" t="s">
         <v>244</v>
       </c>
       <c r="C50" s="88" t="s">
@@ -61701,7 +61740,7 @@
       <c r="A51" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="B51" s="99" t="s">
+      <c r="B51" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C51" s="87" t="s">
@@ -61719,7 +61758,7 @@
       <c r="A52" s="86" t="s">
         <v>271</v>
       </c>
-      <c r="B52" s="98" t="s">
+      <c r="B52" s="96" t="s">
         <v>250</v>
       </c>
       <c r="C52" s="87" t="s">
@@ -61737,7 +61776,7 @@
       <c r="A53" s="86" t="s">
         <v>297</v>
       </c>
-      <c r="B53" s="99" t="s">
+      <c r="B53" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C53" s="87" t="s">
@@ -61755,7 +61794,7 @@
       <c r="A54" s="86" t="s">
         <v>298</v>
       </c>
-      <c r="B54" s="99" t="s">
+      <c r="B54" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C54" s="87" t="s">
@@ -61770,37 +61809,37 @@
       <c r="F54" s="86"/>
     </row>
     <row r="55" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="94" t="s">
+      <c r="A55" s="92" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="101" t="s">
+      <c r="B55" s="99" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="92" t="s">
+      <c r="C55" s="90" t="s">
         <v>200</v>
       </c>
-      <c r="D55" s="93" t="s">
+      <c r="D55" s="91" t="s">
         <v>23</v>
       </c>
-      <c r="E55" s="93" t="s">
+      <c r="E55" s="91" t="s">
         <v>23</v>
       </c>
       <c r="F55" s="86"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="97" t="s">
+      <c r="A56" s="95" t="s">
         <v>224</v>
       </c>
-      <c r="B56" s="104" t="s">
+      <c r="B56" s="102" t="s">
         <v>224</v>
       </c>
-      <c r="C56" s="95" t="s">
+      <c r="C56" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="D56" s="96" t="s">
+      <c r="D56" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="E56" s="97" t="s">
+      <c r="E56" s="95" t="s">
         <v>334</v>
       </c>
       <c r="F56" s="86"/>
@@ -61809,7 +61848,7 @@
       <c r="A57" s="86" t="s">
         <v>288</v>
       </c>
-      <c r="B57" s="98" t="s">
+      <c r="B57" s="96" t="s">
         <v>331</v>
       </c>
       <c r="C57" s="86" t="s">
@@ -61827,7 +61866,7 @@
       <c r="A58" s="86" t="s">
         <v>289</v>
       </c>
-      <c r="B58" s="98" t="s">
+      <c r="B58" s="96" t="s">
         <v>332</v>
       </c>
       <c r="C58" s="86" t="s">
@@ -61845,7 +61884,7 @@
       <c r="A59" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="B59" s="99" t="s">
+      <c r="B59" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C59" s="86" t="s">
@@ -61863,7 +61902,7 @@
       <c r="A60" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="B60" s="98" t="s">
+      <c r="B60" s="96" t="s">
         <v>253</v>
       </c>
       <c r="C60" s="86" t="s">
@@ -61881,7 +61920,7 @@
       <c r="A61" s="86" t="s">
         <v>292</v>
       </c>
-      <c r="B61" s="99" t="s">
+      <c r="B61" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C61" s="86" t="s">
@@ -61899,7 +61938,7 @@
       <c r="A62" s="86" t="s">
         <v>299</v>
       </c>
-      <c r="B62" s="99" t="s">
+      <c r="B62" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C62" s="88" t="s">
@@ -61917,7 +61956,7 @@
       <c r="A63" s="86" t="s">
         <v>296</v>
       </c>
-      <c r="B63" s="99" t="s">
+      <c r="B63" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C63" s="86" t="s">
@@ -61935,7 +61974,7 @@
       <c r="A64" s="86" t="s">
         <v>271</v>
       </c>
-      <c r="B64" s="98" t="s">
+      <c r="B64" s="96" t="s">
         <v>250</v>
       </c>
       <c r="C64" s="86" t="s">
@@ -61953,7 +61992,7 @@
       <c r="A65" s="86" t="s">
         <v>297</v>
       </c>
-      <c r="B65" s="99" t="s">
+      <c r="B65" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C65" s="86" t="s">
@@ -61971,7 +62010,7 @@
       <c r="A66" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="B66" s="98" t="s">
+      <c r="B66" s="96" t="s">
         <v>225</v>
       </c>
       <c r="C66" s="86" t="s">
@@ -61989,7 +62028,7 @@
       <c r="A67" s="86" t="s">
         <v>269</v>
       </c>
-      <c r="B67" s="99" t="s">
+      <c r="B67" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C67" s="86" t="s">
@@ -62007,7 +62046,7 @@
       <c r="A68" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="B68" s="98" t="s">
+      <c r="B68" s="96" t="s">
         <v>254</v>
       </c>
       <c r="C68" s="86" t="s">
@@ -62022,132 +62061,183 @@
       <c r="F68" s="86"/>
     </row>
     <row r="69" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="94" t="s">
+      <c r="A69" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="B69" s="101" t="s">
+      <c r="B69" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C69" s="94" t="s">
+      <c r="C69" s="86" t="s">
         <v>255</v>
       </c>
-      <c r="D69" s="93" t="s">
+      <c r="D69" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="E69" s="93" t="s">
+      <c r="E69" s="88" t="s">
         <v>23</v>
       </c>
       <c r="F69" s="86"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="90" t="s">
+      <c r="A70" s="122" t="s">
         <v>337</v>
       </c>
-      <c r="B70" s="105" t="s">
+      <c r="B70" s="94" t="s">
+        <v>338</v>
+      </c>
+      <c r="C70" s="123" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70" s="93" t="s">
+        <v>214</v>
+      </c>
+      <c r="E70" s="124" t="s">
         <v>23</v>
       </c>
-      <c r="C70" s="91" t="s">
+      <c r="F70" s="86"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A71" s="113" t="s">
+        <v>262</v>
+      </c>
+      <c r="B71" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D70" s="90" t="s">
-        <v>70</v>
-      </c>
-      <c r="E70" s="91" t="s">
+      <c r="C71" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="F70" s="86"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="86" t="s">
-        <v>214</v>
-      </c>
-      <c r="B71" s="99" t="s">
+      <c r="D71" s="86" t="s">
+        <v>313</v>
+      </c>
+      <c r="E71" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C71" s="88" t="s">
+      <c r="F71" s="86"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A72" s="113" t="s">
+        <v>339</v>
+      </c>
+      <c r="B72" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D71" s="86" t="s">
-        <v>214</v>
-      </c>
-      <c r="E71" s="88" t="s">
+      <c r="C72" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="F71" s="86"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="86" t="s">
-        <v>215</v>
-      </c>
-      <c r="B72" s="99" t="s">
+      <c r="D72" s="86" t="s">
+        <v>339</v>
+      </c>
+      <c r="E72" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C72" s="88" t="s">
+      <c r="F72" s="86"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A73" s="113" t="s">
+        <v>225</v>
+      </c>
+      <c r="B73" s="112" t="s">
+        <v>225</v>
+      </c>
+      <c r="C73" s="117" t="s">
+        <v>225</v>
+      </c>
+      <c r="D73" s="86" t="s">
+        <v>225</v>
+      </c>
+      <c r="E73" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="D72" s="86" t="s">
-        <v>215</v>
-      </c>
-      <c r="E72" s="88" t="s">
+      <c r="F73" s="86"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A74" s="113" t="s">
+        <v>255</v>
+      </c>
+      <c r="B74" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="F72" s="86"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="B73" s="99" t="s">
+      <c r="C74" s="118" t="s">
+        <v>255</v>
+      </c>
+      <c r="D74" s="86" t="s">
+        <v>255</v>
+      </c>
+      <c r="E74" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="C73" s="88" t="s">
+      <c r="F74" s="86"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A75" s="113" t="s">
+        <v>296</v>
+      </c>
+      <c r="B75" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D73" s="86" t="s">
-        <v>216</v>
-      </c>
-      <c r="E73" s="88" t="s">
+      <c r="C75" s="113" t="s">
+        <v>124</v>
+      </c>
+      <c r="D75" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="F73" s="86"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" s="99" t="s">
+      <c r="E75" s="119"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A76" s="113" t="s">
+        <v>271</v>
+      </c>
+      <c r="B76" s="112" t="s">
+        <v>250</v>
+      </c>
+      <c r="C76" s="113" t="s">
+        <v>126</v>
+      </c>
+      <c r="D76" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="88" t="s">
+      <c r="E76" s="119"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A77" s="113" t="s">
+        <v>297</v>
+      </c>
+      <c r="B77" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="D74" s="86" t="s">
-        <v>217</v>
-      </c>
-      <c r="E74" s="88" t="s">
+      <c r="C77" s="113" t="s">
+        <v>128</v>
+      </c>
+      <c r="D77" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="F74" s="86"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="86" t="s">
-        <v>218</v>
-      </c>
-      <c r="B75" s="99" t="s">
+      <c r="E77" s="119"/>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A78" s="113" t="s">
+        <v>269</v>
+      </c>
+      <c r="B78" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C75" s="87"/>
-      <c r="D75" s="86" t="s">
-        <v>218</v>
-      </c>
-      <c r="E75" s="88" t="s">
-        <v>23</v>
-      </c>
-      <c r="F75" s="86"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="40"/>
-      <c r="B76" s="40"/>
+      <c r="C78" s="113" t="s">
+        <v>269</v>
+      </c>
+      <c r="D78" s="40"/>
+      <c r="E78" s="119"/>
+    </row>
+    <row r="79" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="114" t="s">
+        <v>226</v>
+      </c>
+      <c r="B79" s="115" t="s">
+        <v>254</v>
+      </c>
+      <c r="C79" s="114" t="s">
+        <v>226</v>
+      </c>
+      <c r="D79" s="120"/>
+      <c r="E79" s="121"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add stereotypes to excel comparison
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Papers\ECMFA_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B17188F-798E-433B-9F49-6AFE1BDE04E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFE2B4C-A9F8-419D-AF55-9D1B1F7FECEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="17520" windowHeight="12600" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="354">
   <si>
     <t>Vergleichskriterien/Features</t>
   </si>
@@ -1061,6 +1061,48 @@
   <si>
     <t>multiple</t>
   </si>
+  <si>
+    <t>abstracted from returnType + parameters</t>
+  </si>
+  <si>
+    <t>minMultiplicity &gt; 1</t>
+  </si>
+  <si>
+    <t>map to parameters.unitOfMeasurement</t>
+  </si>
+  <si>
+    <t>VersionableElement</t>
+  </si>
+  <si>
+    <t>DTClass</t>
+  </si>
+  <si>
+    <t>DTProperty.isTimeSeries</t>
+  </si>
+  <si>
+    <t>DTProperty.isFault</t>
+  </si>
+  <si>
+    <t>DTProperty</t>
+  </si>
+  <si>
+    <t>readOnly=false</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>'map to parameters.languageVErsion</t>
+  </si>
+  <si>
+    <t>Association.Properties</t>
+  </si>
+  <si>
+    <t>MemberEnd.lower&gt;1</t>
+  </si>
+  <si>
+    <t>MemberEnd.upper&gt;1</t>
+  </si>
 </sst>
 </file>
 
@@ -1157,7 +1199,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1174,6 +1216,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1583,7 +1631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1799,6 +1847,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="32" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="31" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -60829,8 +60884,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81660679-4C16-4328-828C-2DD56627BD9C}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -60901,7 +60956,7 @@
         <v>269</v>
       </c>
       <c r="B4" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C4" s="87" t="s">
         <v>269</v>
@@ -60991,7 +61046,7 @@
         <v>297</v>
       </c>
       <c r="B9" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C9" s="87" t="s">
         <v>128</v>
@@ -61009,7 +61064,7 @@
         <v>272</v>
       </c>
       <c r="B10" s="97" t="s">
-        <v>23</v>
+        <v>344</v>
       </c>
       <c r="C10" s="88" t="s">
         <v>23</v>
@@ -61027,7 +61082,7 @@
         <v>258</v>
       </c>
       <c r="B11" s="97" t="s">
-        <v>23</v>
+        <v>344</v>
       </c>
       <c r="C11" s="88" t="s">
         <v>23</v>
@@ -61063,7 +61118,7 @@
         <v>336</v>
       </c>
       <c r="B13" s="97" t="s">
-        <v>23</v>
+        <v>344</v>
       </c>
       <c r="C13" s="87"/>
       <c r="D13" s="87" t="s">
@@ -61131,7 +61186,7 @@
         <v>294</v>
       </c>
       <c r="B17" s="97" t="s">
-        <v>23</v>
+        <v>346</v>
       </c>
       <c r="C17" s="88" t="s">
         <v>23</v>
@@ -61148,7 +61203,9 @@
       <c r="A18" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="B18" s="101"/>
+      <c r="B18" s="101" t="s">
+        <v>345</v>
+      </c>
       <c r="C18" s="87" t="s">
         <v>61</v>
       </c>
@@ -61179,11 +61236,11 @@
       <c r="F19" s="86"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="86" t="s">
+      <c r="A20" s="125" t="s">
         <v>274</v>
       </c>
       <c r="B20" s="97" t="s">
-        <v>23</v>
+        <v>347</v>
       </c>
       <c r="C20" s="88" t="s">
         <v>23</v>
@@ -61201,7 +61258,7 @@
         <v>275</v>
       </c>
       <c r="B21" s="97" t="s">
-        <v>23</v>
+        <v>347</v>
       </c>
       <c r="C21" s="88" t="s">
         <v>23</v>
@@ -61219,7 +61276,7 @@
         <v>262</v>
       </c>
       <c r="B22" s="97" t="s">
-        <v>23</v>
+        <v>341</v>
       </c>
       <c r="C22" s="88" t="s">
         <v>23</v>
@@ -61255,7 +61312,7 @@
         <v>276</v>
       </c>
       <c r="B24" s="97" t="s">
-        <v>23</v>
+        <v>348</v>
       </c>
       <c r="C24" s="88" t="s">
         <v>23</v>
@@ -61273,7 +61330,7 @@
         <v>277</v>
       </c>
       <c r="B25" s="97" t="s">
-        <v>23</v>
+        <v>349</v>
       </c>
       <c r="C25" s="87" t="s">
         <v>317</v>
@@ -61291,7 +61348,7 @@
         <v>255</v>
       </c>
       <c r="B26" s="96" t="s">
-        <v>226</v>
+        <v>343</v>
       </c>
       <c r="C26" s="87" t="s">
         <v>255</v>
@@ -61341,7 +61398,7 @@
       <c r="F28" s="86"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="86" t="s">
+      <c r="A29" s="125" t="s">
         <v>273</v>
       </c>
       <c r="B29" s="96" t="s">
@@ -61381,7 +61438,7 @@
         <v>280</v>
       </c>
       <c r="B31" s="97" t="s">
-        <v>23</v>
+        <v>347</v>
       </c>
       <c r="C31" s="87" t="s">
         <v>321</v>
@@ -61417,7 +61474,7 @@
         <v>269</v>
       </c>
       <c r="B33" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C33" s="87" t="s">
         <v>269</v>
@@ -61453,7 +61510,7 @@
         <v>296</v>
       </c>
       <c r="B35" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C35" s="87" t="s">
         <v>124</v>
@@ -61489,7 +61546,7 @@
         <v>297</v>
       </c>
       <c r="B37" s="99" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C37" s="90" t="s">
         <v>128</v>
@@ -61560,8 +61617,8 @@
       <c r="A41" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="B41" s="97" t="s">
-        <v>23</v>
+      <c r="B41" s="126" t="s">
+        <v>340</v>
       </c>
       <c r="C41" s="88" t="s">
         <v>23</v>
@@ -61596,8 +61653,8 @@
       <c r="A43" s="86" t="s">
         <v>262</v>
       </c>
-      <c r="B43" s="97" t="s">
-        <v>23</v>
+      <c r="B43" s="126" t="s">
+        <v>170</v>
       </c>
       <c r="C43" s="88" t="s">
         <v>23</v>
@@ -61615,7 +61672,7 @@
         <v>286</v>
       </c>
       <c r="B44" s="97" t="s">
-        <v>23</v>
+        <v>170</v>
       </c>
       <c r="C44" s="88" t="s">
         <v>23</v>
@@ -61651,7 +61708,7 @@
         <v>255</v>
       </c>
       <c r="B46" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C46" s="87" t="s">
         <v>270</v>
@@ -61669,7 +61726,7 @@
         <v>269</v>
       </c>
       <c r="B47" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C47" s="87" t="s">
         <v>269</v>
@@ -61741,7 +61798,7 @@
         <v>296</v>
       </c>
       <c r="B51" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C51" s="87" t="s">
         <v>124</v>
@@ -61777,7 +61834,7 @@
         <v>297</v>
       </c>
       <c r="B53" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C53" s="87" t="s">
         <v>330</v>
@@ -61795,7 +61852,7 @@
         <v>298</v>
       </c>
       <c r="B54" s="97" t="s">
-        <v>23</v>
+        <v>350</v>
       </c>
       <c r="C54" s="87" t="s">
         <v>110</v>
@@ -61812,8 +61869,8 @@
       <c r="A55" s="92" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="99" t="s">
-        <v>23</v>
+      <c r="B55" s="127" t="s">
+        <v>342</v>
       </c>
       <c r="C55" s="90" t="s">
         <v>200</v>
@@ -61885,7 +61942,7 @@
         <v>290</v>
       </c>
       <c r="B59" s="97" t="s">
-        <v>23</v>
+        <v>351</v>
       </c>
       <c r="C59" s="86" t="s">
         <v>290</v>
@@ -61957,7 +62014,7 @@
         <v>296</v>
       </c>
       <c r="B63" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C63" s="86" t="s">
         <v>124</v>
@@ -61993,7 +62050,7 @@
         <v>297</v>
       </c>
       <c r="B65" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C65" s="86" t="s">
         <v>128</v>
@@ -62029,7 +62086,7 @@
         <v>269</v>
       </c>
       <c r="B67" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C67" s="86" t="s">
         <v>269</v>
@@ -62065,7 +62122,7 @@
         <v>255</v>
       </c>
       <c r="B69" s="97" t="s">
-        <v>23</v>
+        <v>343</v>
       </c>
       <c r="C69" s="86" t="s">
         <v>255</v>
@@ -62101,7 +62158,7 @@
         <v>262</v>
       </c>
       <c r="B71" s="88" t="s">
-        <v>23</v>
+        <v>352</v>
       </c>
       <c r="C71" s="116" t="s">
         <v>23</v>
@@ -62119,7 +62176,7 @@
         <v>339</v>
       </c>
       <c r="B72" s="88" t="s">
-        <v>23</v>
+        <v>353</v>
       </c>
       <c r="C72" s="116" t="s">
         <v>23</v>
@@ -62154,8 +62211,8 @@
       <c r="A74" s="113" t="s">
         <v>255</v>
       </c>
-      <c r="B74" s="88" t="s">
-        <v>23</v>
+      <c r="B74" s="97" t="s">
+        <v>343</v>
       </c>
       <c r="C74" s="118" t="s">
         <v>255</v>
@@ -62172,8 +62229,8 @@
       <c r="A75" s="113" t="s">
         <v>296</v>
       </c>
-      <c r="B75" s="88" t="s">
-        <v>23</v>
+      <c r="B75" s="97" t="s">
+        <v>343</v>
       </c>
       <c r="C75" s="113" t="s">
         <v>124</v>
@@ -62202,8 +62259,8 @@
       <c r="A77" s="113" t="s">
         <v>297</v>
       </c>
-      <c r="B77" s="88" t="s">
-        <v>23</v>
+      <c r="B77" s="97" t="s">
+        <v>343</v>
       </c>
       <c r="C77" s="113" t="s">
         <v>128</v>
@@ -62217,8 +62274,8 @@
       <c r="A78" s="113" t="s">
         <v>269</v>
       </c>
-      <c r="B78" s="88" t="s">
-        <v>23</v>
+      <c r="B78" s="97" t="s">
+        <v>343</v>
       </c>
       <c r="C78" s="113" t="s">
         <v>269</v>

</xml_diff>